<commit_message>
Botão buscar e filtro por especialidade
</commit_message>
<xml_diff>
--- a/enderecos_com_cep_latlong.xlsx
+++ b/enderecos_com_cep_latlong.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brunomelo\Buscar_cep\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8BAD05-2B10-43A5-82E6-5F701FD0734A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-19310" yWindow="4670" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="344">
   <si>
-    <t>NOM E DO PRESTADOR</t>
-  </si>
-  <si>
     <t>ESPECIALIDADE</t>
   </si>
   <si>
@@ -1046,13 +1049,16 @@
   </si>
   <si>
     <t>21351-080</t>
+  </si>
+  <si>
+    <t>NOME DO PRESTADOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1123,18 +1129,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1172,7 +1186,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1206,6 +1220,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1240,9 +1255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1415,909 +1431,909 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2">
         <v>1059</v>
       </c>
       <c r="F2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L2">
-        <v>-22.7015081</v>
+        <v>-22.701508100000002</v>
       </c>
       <c r="M2">
-        <v>-43.563591</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>-43.563591000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>302</v>
       </c>
       <c r="F3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L3">
         <v>-22.9516977</v>
       </c>
       <c r="M3">
-        <v>-43.1904336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>-43.190433599999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4">
         <v>183</v>
       </c>
       <c r="F4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L4">
-        <v>-22.9577266</v>
+        <v>-22.957726600000001</v>
       </c>
       <c r="M4">
-        <v>-43.1902102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>-43.190210200000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>375</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L6">
-        <v>-22.8968192</v>
+        <v>-22.896819199999999</v>
       </c>
       <c r="M6">
-        <v>-43.5616562</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>-43.561656200000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7">
         <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L7">
-        <v>-22.9070846</v>
+        <v>-22.907084600000001</v>
       </c>
       <c r="M7">
-        <v>-43.175924</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>-43.175924000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>190</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L8">
-        <v>-22.9509086</v>
+        <v>-22.950908600000002</v>
       </c>
       <c r="M8">
-        <v>-43.1829287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>-43.182928699999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9">
         <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L9">
-        <v>-22.9509086</v>
+        <v>-22.950908600000002</v>
       </c>
       <c r="M9">
-        <v>-43.1829287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>-43.182928699999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10">
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L10">
-        <v>-22.9288655</v>
+        <v>-22.928865500000001</v>
       </c>
       <c r="M10">
-        <v>-43.2338789</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>-43.233878900000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11">
         <v>111</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L11">
         <v>-22.8819531</v>
       </c>
       <c r="M11">
-        <v>-43.4636044</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>-43.463604400000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12">
         <v>500</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L12">
-        <v>-22.9647074</v>
+        <v>-22.964707400000002</v>
       </c>
       <c r="M12">
         <v>-43.1758229</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>660</v>
       </c>
       <c r="G13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L13">
-        <v>-22.9659065</v>
+        <v>-22.965906499999999</v>
       </c>
       <c r="M13">
-        <v>-43.2189688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>-43.218968799999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14">
         <v>3600</v>
       </c>
       <c r="F14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L14">
-        <v>-22.9076987</v>
+        <v>-22.907698700000001</v>
       </c>
       <c r="M14">
-        <v>-43.5657515</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>-43.565751499999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15">
         <v>3500</v>
       </c>
       <c r="F15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16">
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17">
         <v>674</v>
       </c>
       <c r="F17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L17">
-        <v>-22.9659065</v>
+        <v>-22.965906499999999</v>
       </c>
       <c r="M17">
-        <v>-43.2189688</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>-43.218968799999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18">
         <v>232</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L18">
-        <v>-22.9243493</v>
+        <v>-22.924349299999999</v>
       </c>
       <c r="M18">
-        <v>-43.2240065</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>-43.224006500000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19">
         <v>210</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L19">
         <v>-22.9207459</v>
       </c>
       <c r="M19">
-        <v>-43.2175742</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>-43.217574200000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20">
         <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L20">
-        <v>-22.9112626</v>
+        <v>-22.911262600000001</v>
       </c>
       <c r="M20">
         <v>-43.1781413</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E21">
         <v>2480</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L21">
-        <v>-22.9986834</v>
+        <v>-22.998683400000001</v>
       </c>
       <c r="M21">
-        <v>-43.3639997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>-43.363999700000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22">
         <v>99</v>
       </c>
       <c r="F22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L22">
         <v>-22.873224</v>
       </c>
       <c r="M22">
-        <v>-43.3390683</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>-43.339068300000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L23">
         <v>-22.9670734</v>
@@ -2326,504 +2342,504 @@
         <v>-43.2184539</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24">
         <v>260</v>
       </c>
       <c r="F24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L24">
-        <v>-22.905912</v>
+        <v>-22.905912000000001</v>
       </c>
       <c r="M24">
-        <v>-43.5657236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>-43.565723599999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25">
         <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L25">
-        <v>-22.9249187</v>
+        <v>-22.924918699999999</v>
       </c>
       <c r="M25">
-        <v>-43.2323149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>-43.232314899999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26">
         <v>351</v>
       </c>
       <c r="F26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L26">
-        <v>-22.984037</v>
+        <v>-22.984037000000001</v>
       </c>
       <c r="M26">
-        <v>-43.2087552</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>-43.208755199999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E27">
         <v>351</v>
       </c>
       <c r="F27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L27">
-        <v>-22.984037</v>
+        <v>-22.984037000000001</v>
       </c>
       <c r="M27">
-        <v>-43.2087552</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>-43.208755199999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28">
         <v>2251</v>
       </c>
       <c r="G28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L28">
-        <v>-22.9986834</v>
+        <v>-22.998683400000001</v>
       </c>
       <c r="M28">
-        <v>-43.3639997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>-43.363999700000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E29">
         <v>228</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L29">
         <v>-22.9454037</v>
       </c>
       <c r="M29">
-        <v>-43.180818</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>-43.180818000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30">
         <v>130</v>
       </c>
       <c r="G30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L30">
-        <v>-22.8968192</v>
+        <v>-22.896819199999999</v>
       </c>
       <c r="M30">
-        <v>-43.5616562</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>-43.561656200000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31">
         <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L31">
         <v>-22.9759955</v>
       </c>
       <c r="M31">
-        <v>-43.2285129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+        <v>-43.228512899999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E32">
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E33">
         <v>550</v>
       </c>
       <c r="F33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L33">
-        <v>-22.9943301</v>
+        <v>-22.994330099999999</v>
       </c>
       <c r="M33">
-        <v>-43.4031123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>-43.403112299999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34">
         <v>27</v>
       </c>
       <c r="G34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L34">
-        <v>-22.9569013</v>
+        <v>-22.956901299999998</v>
       </c>
       <c r="M34">
         <v>-43.1962726</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35">
         <v>105</v>
       </c>
       <c r="G35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L35">
-        <v>-22.8968192</v>
+        <v>-22.896819199999999</v>
       </c>
       <c r="M35">
-        <v>-43.5616562</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+        <v>-43.561656200000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36">
         <v>67</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L36">
         <v>-22.9466532</v>
@@ -2832,916 +2848,916 @@
         <v>-43.1883312</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37">
         <v>3255</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L37">
-        <v>-22.9986834</v>
+        <v>-22.998683400000001</v>
       </c>
       <c r="M37">
-        <v>-43.3639997</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>-43.363999700000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E38">
         <v>173</v>
       </c>
       <c r="F38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L38">
         <v>-22.9017974</v>
       </c>
       <c r="M38">
-        <v>-43.1789278</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>-43.178927799999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E39">
         <v>1054</v>
       </c>
       <c r="G39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E40">
         <v>151</v>
       </c>
       <c r="F40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L40">
-        <v>-22.9035822</v>
+        <v>-22.903582199999999</v>
       </c>
       <c r="M40">
         <v>-43.1792783</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E41">
         <v>201</v>
       </c>
       <c r="G41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L41">
-        <v>-22.9734814</v>
+        <v>-22.973481400000001</v>
       </c>
       <c r="M41">
-        <v>-43.3822898</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>-43.382289800000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E42">
         <v>144</v>
       </c>
       <c r="G42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L42">
-        <v>-22.924473</v>
+        <v>-22.924472999999999</v>
       </c>
       <c r="M42">
-        <v>-43.236765</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>-43.236764999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43">
         <v>144</v>
       </c>
       <c r="F43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L43">
-        <v>-22.9697708</v>
+        <v>-22.969770799999999</v>
       </c>
       <c r="M43">
-        <v>-43.1863868</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>-43.186386800000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E44">
         <v>464</v>
       </c>
       <c r="F44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L44">
         <v>-22.9516977</v>
       </c>
       <c r="M44">
-        <v>-43.1904336</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+        <v>-43.190433599999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E45">
         <v>70</v>
       </c>
       <c r="G45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L45">
         <v>-22.9209022</v>
       </c>
       <c r="M45">
-        <v>-43.2150458</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+        <v>-43.215045799999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E46">
         <v>2600</v>
       </c>
       <c r="F46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L46">
-        <v>-23.0066084</v>
+        <v>-23.006608400000001</v>
       </c>
       <c r="M46">
-        <v>-43.3660606</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>-43.366060599999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E47">
         <v>515</v>
       </c>
       <c r="G47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L47">
         <v>-22.8819531</v>
       </c>
       <c r="M47">
-        <v>-43.4636044</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+        <v>-43.463604400000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48">
         <v>1079</v>
       </c>
       <c r="G48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L48">
         <v>-22.9384853</v>
       </c>
       <c r="M48">
-        <v>-43.3479622</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>-43.347962199999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E49">
         <v>668</v>
       </c>
       <c r="F49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L49">
-        <v>-22.795898</v>
+        <v>-22.795898000000001</v>
       </c>
       <c r="M49">
-        <v>-43.1974295</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>-43.197429499999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E50">
         <v>295</v>
       </c>
       <c r="G50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L50">
-        <v>-22.9280712</v>
+        <v>-22.928071200000002</v>
       </c>
       <c r="M50">
-        <v>-43.2301488</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>-43.230148800000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E51">
         <v>131</v>
       </c>
       <c r="G51" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" t="s">
+        <v>233</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K51" t="s">
+        <v>335</v>
+      </c>
+      <c r="L51">
+        <v>-22.928371899999998</v>
+      </c>
+      <c r="M51">
+        <v>-43.684195799999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" t="s">
+        <v>147</v>
+      </c>
+      <c r="G52" t="s">
         <v>208</v>
       </c>
-      <c r="H51" t="s">
-        <v>234</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="H52" t="s">
+        <v>237</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K52" t="s">
         <v>336</v>
       </c>
-      <c r="L51">
-        <v>-22.9283719</v>
-      </c>
-      <c r="M51">
-        <v>-43.6841958</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" t="s">
+      <c r="L52">
+        <v>-22.965530099999999</v>
+      </c>
+      <c r="M52">
+        <v>-43.276316000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>37</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>76</v>
       </c>
-      <c r="C52" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" t="s">
         <v>139</v>
-      </c>
-      <c r="E52" t="s">
-        <v>148</v>
-      </c>
-      <c r="G52" t="s">
-        <v>209</v>
-      </c>
-      <c r="H52" t="s">
-        <v>238</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="K52" t="s">
-        <v>337</v>
-      </c>
-      <c r="L52">
-        <v>-22.9655301</v>
-      </c>
-      <c r="M52">
-        <v>-43.276316</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" t="s">
-        <v>140</v>
       </c>
       <c r="E53">
         <v>500</v>
       </c>
       <c r="F53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L53">
-        <v>-23.0003774</v>
+        <v>-23.000377400000001</v>
       </c>
       <c r="M53">
-        <v>-43.33557</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>-43.335569999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E54">
         <v>155</v>
       </c>
       <c r="F54" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L54">
-        <v>-23.007138</v>
+        <v>-23.007138000000001</v>
       </c>
       <c r="M54">
-        <v>-43.3102663</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+        <v>-43.310266300000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E55">
         <v>500</v>
       </c>
       <c r="F55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L55">
-        <v>-23.0003774</v>
+        <v>-23.000377400000001</v>
       </c>
       <c r="M55">
-        <v>-43.33557</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+        <v>-43.335569999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E56">
         <v>23</v>
       </c>
       <c r="G56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L56">
-        <v>-22.8972514</v>
+        <v>-22.897251399999998</v>
       </c>
       <c r="M56">
-        <v>-43.2791713</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+        <v>-43.279171300000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E57">
         <v>49</v>
       </c>
       <c r="G57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K57" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L57">
-        <v>-22.9403485</v>
+        <v>-22.940348499999999</v>
       </c>
       <c r="M57">
-        <v>-43.1813178</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+        <v>-43.181317800000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E58">
         <v>153</v>
       </c>
       <c r="G58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L58">
-        <v>-22.8982503</v>
+        <v>-22.898250300000001</v>
       </c>
       <c r="M58">
-        <v>-43.2259001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+        <v>-43.225900099999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E59">
         <v>2480</v>
       </c>
       <c r="F59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L59">
-        <v>-23.0003774</v>
+        <v>-23.000377400000001</v>
       </c>
       <c r="M59">
-        <v>-43.33557</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+        <v>-43.335569999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E60">
         <v>156</v>
@@ -3750,112 +3766,112 @@
         <v>2609</v>
       </c>
       <c r="G60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K60" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L60">
         <v>-22.9017974</v>
       </c>
       <c r="M60">
-        <v>-43.1789278</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>-43.178927799999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E61">
         <v>500</v>
       </c>
       <c r="F61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L61">
-        <v>-23.0003774</v>
+        <v>-23.000377400000001</v>
       </c>
       <c r="M61">
-        <v>-43.33557</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+        <v>-43.335569999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E62">
         <v>1000</v>
       </c>
       <c r="F62" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E63">
         <v>112</v>
@@ -3864,39 +3880,39 @@
         <v>610</v>
       </c>
       <c r="G63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L63">
-        <v>-22.9243493</v>
+        <v>-22.924349299999999</v>
       </c>
       <c r="M63">
-        <v>-43.2240065</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>-43.224006500000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E64">
         <v>105</v>
@@ -3905,39 +3921,39 @@
         <v>108</v>
       </c>
       <c r="G64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L64">
-        <v>-22.9256059</v>
+        <v>-22.925605900000001</v>
       </c>
       <c r="M64">
         <v>-43.2274314</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E65">
         <v>647</v>
@@ -3946,39 +3962,39 @@
         <v>802</v>
       </c>
       <c r="G65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L65">
-        <v>-22.9647074</v>
+        <v>-22.964707400000002</v>
       </c>
       <c r="M65">
         <v>-43.1758229</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E66">
         <v>142</v>
@@ -3987,311 +4003,311 @@
         <v>610</v>
       </c>
       <c r="G66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H66" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K66" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L66">
         <v>-22.8701981</v>
       </c>
       <c r="M66">
-        <v>-43.3396644</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+        <v>-43.339664399999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E67">
         <v>27</v>
       </c>
       <c r="G67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K67" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L67">
-        <v>-22.9569013</v>
+        <v>-22.956901299999998</v>
       </c>
       <c r="M67">
         <v>-43.1962726</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E68">
         <v>105</v>
       </c>
       <c r="G68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K68" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L68">
-        <v>-22.8968192</v>
+        <v>-22.896819199999999</v>
       </c>
       <c r="M68">
-        <v>-43.5616562</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+        <v>-43.561656200000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
         <v>84</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
-      <c r="A70" t="s">
-        <v>47</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" t="s">
         <v>85</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
-      <c r="A71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" t="s">
         <v>86</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
-      <c r="A72" t="s">
-        <v>47</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" t="s">
         <v>87</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
-      <c r="A73" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" t="s">
         <v>88</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
-      <c r="A74" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>46</v>
+      </c>
+      <c r="B75" t="s">
         <v>89</v>
       </c>
-      <c r="C74" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" t="s">
-        <v>47</v>
-      </c>
-      <c r="B75" t="s">
-        <v>90</v>
-      </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="J4" r:id="rId4"/>
-    <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="J5" r:id="rId6"/>
-    <hyperlink ref="I6" r:id="rId7"/>
-    <hyperlink ref="J6" r:id="rId8"/>
-    <hyperlink ref="I7" r:id="rId9"/>
-    <hyperlink ref="J7" r:id="rId10"/>
-    <hyperlink ref="I8" r:id="rId11"/>
-    <hyperlink ref="J8" r:id="rId12"/>
-    <hyperlink ref="I9" r:id="rId13"/>
-    <hyperlink ref="J9" r:id="rId14"/>
-    <hyperlink ref="I10" r:id="rId15"/>
-    <hyperlink ref="I11" r:id="rId16"/>
-    <hyperlink ref="J11" r:id="rId17"/>
-    <hyperlink ref="I12" r:id="rId18"/>
-    <hyperlink ref="J12" r:id="rId19"/>
-    <hyperlink ref="I13" r:id="rId20"/>
-    <hyperlink ref="J13" r:id="rId21"/>
-    <hyperlink ref="I14" r:id="rId22"/>
-    <hyperlink ref="J14" r:id="rId23"/>
-    <hyperlink ref="I15" r:id="rId24"/>
-    <hyperlink ref="J15" r:id="rId25"/>
-    <hyperlink ref="I16" r:id="rId26"/>
-    <hyperlink ref="J16" r:id="rId27"/>
-    <hyperlink ref="I17" r:id="rId28"/>
-    <hyperlink ref="J17" r:id="rId29"/>
-    <hyperlink ref="I18" r:id="rId30"/>
-    <hyperlink ref="J18" r:id="rId31"/>
-    <hyperlink ref="I19" r:id="rId32"/>
-    <hyperlink ref="J19" r:id="rId33"/>
-    <hyperlink ref="I20" r:id="rId34"/>
-    <hyperlink ref="J20" r:id="rId35"/>
-    <hyperlink ref="I21" r:id="rId36"/>
-    <hyperlink ref="J21" r:id="rId37"/>
-    <hyperlink ref="I22" r:id="rId38"/>
-    <hyperlink ref="J22" r:id="rId39"/>
-    <hyperlink ref="I23" r:id="rId40"/>
-    <hyperlink ref="J23" r:id="rId41"/>
-    <hyperlink ref="I24" r:id="rId42"/>
-    <hyperlink ref="J24" r:id="rId43"/>
-    <hyperlink ref="I25" r:id="rId44"/>
-    <hyperlink ref="J25" r:id="rId45"/>
-    <hyperlink ref="I26" r:id="rId46"/>
-    <hyperlink ref="J26" r:id="rId47"/>
-    <hyperlink ref="I27" r:id="rId48"/>
-    <hyperlink ref="J27" r:id="rId49"/>
-    <hyperlink ref="I28" r:id="rId50"/>
-    <hyperlink ref="J28" r:id="rId51"/>
-    <hyperlink ref="I29" r:id="rId52"/>
-    <hyperlink ref="J29" r:id="rId53"/>
-    <hyperlink ref="I30" r:id="rId54"/>
-    <hyperlink ref="J30" r:id="rId55"/>
-    <hyperlink ref="I31" r:id="rId56"/>
-    <hyperlink ref="J31" r:id="rId57"/>
-    <hyperlink ref="I32" r:id="rId58"/>
-    <hyperlink ref="J32" r:id="rId59"/>
-    <hyperlink ref="I33" r:id="rId60"/>
-    <hyperlink ref="J33" r:id="rId61"/>
-    <hyperlink ref="I34" r:id="rId62"/>
-    <hyperlink ref="J34" r:id="rId63"/>
-    <hyperlink ref="I35" r:id="rId64"/>
-    <hyperlink ref="J35" r:id="rId65"/>
-    <hyperlink ref="I36" r:id="rId66"/>
-    <hyperlink ref="J36" r:id="rId67"/>
-    <hyperlink ref="I37" r:id="rId68"/>
-    <hyperlink ref="J37" r:id="rId69"/>
-    <hyperlink ref="I38" r:id="rId70"/>
-    <hyperlink ref="J38" r:id="rId71"/>
-    <hyperlink ref="I39" r:id="rId72"/>
-    <hyperlink ref="J39" r:id="rId73"/>
-    <hyperlink ref="I40" r:id="rId74"/>
-    <hyperlink ref="J40" r:id="rId75"/>
-    <hyperlink ref="I41" r:id="rId76"/>
-    <hyperlink ref="J41" r:id="rId77"/>
-    <hyperlink ref="I42" r:id="rId78"/>
-    <hyperlink ref="J42" r:id="rId79"/>
-    <hyperlink ref="I43" r:id="rId80"/>
-    <hyperlink ref="J43" r:id="rId81"/>
-    <hyperlink ref="I44" r:id="rId82"/>
-    <hyperlink ref="J44" r:id="rId83"/>
-    <hyperlink ref="I45" r:id="rId84"/>
-    <hyperlink ref="J45" r:id="rId85"/>
-    <hyperlink ref="I46" r:id="rId86"/>
-    <hyperlink ref="J46" r:id="rId87"/>
-    <hyperlink ref="I47" r:id="rId88"/>
-    <hyperlink ref="J47" r:id="rId89"/>
-    <hyperlink ref="I48" r:id="rId90"/>
-    <hyperlink ref="J48" r:id="rId91"/>
-    <hyperlink ref="I49" r:id="rId92"/>
-    <hyperlink ref="J49" r:id="rId93"/>
-    <hyperlink ref="I50" r:id="rId94"/>
-    <hyperlink ref="J50" r:id="rId95"/>
-    <hyperlink ref="I51" r:id="rId96"/>
-    <hyperlink ref="J51" r:id="rId97"/>
-    <hyperlink ref="I52" r:id="rId98"/>
-    <hyperlink ref="J52" r:id="rId99"/>
-    <hyperlink ref="I53" r:id="rId100"/>
-    <hyperlink ref="J53" r:id="rId101"/>
-    <hyperlink ref="I54" r:id="rId102"/>
-    <hyperlink ref="J54" r:id="rId103"/>
-    <hyperlink ref="I55" r:id="rId104"/>
-    <hyperlink ref="J55" r:id="rId105"/>
-    <hyperlink ref="I56" r:id="rId106"/>
-    <hyperlink ref="J56" r:id="rId107"/>
-    <hyperlink ref="I57" r:id="rId108"/>
-    <hyperlink ref="J57" r:id="rId109"/>
-    <hyperlink ref="I58" r:id="rId110"/>
-    <hyperlink ref="J58" r:id="rId111"/>
-    <hyperlink ref="I60" r:id="rId112"/>
-    <hyperlink ref="J60" r:id="rId113"/>
-    <hyperlink ref="I61" r:id="rId114"/>
-    <hyperlink ref="J61" r:id="rId115"/>
-    <hyperlink ref="I62" r:id="rId116"/>
-    <hyperlink ref="J62" r:id="rId117"/>
-    <hyperlink ref="I63" r:id="rId118"/>
-    <hyperlink ref="J63" r:id="rId119"/>
-    <hyperlink ref="I64" r:id="rId120"/>
-    <hyperlink ref="J64" r:id="rId121"/>
-    <hyperlink ref="I65" r:id="rId122"/>
-    <hyperlink ref="J65" r:id="rId123"/>
-    <hyperlink ref="I66" r:id="rId124"/>
-    <hyperlink ref="J66" r:id="rId125"/>
-    <hyperlink ref="I67" r:id="rId126"/>
-    <hyperlink ref="J67" r:id="rId127"/>
-    <hyperlink ref="I68" r:id="rId128"/>
-    <hyperlink ref="J68" r:id="rId129"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J13" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="I14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="I15" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="I16" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J16" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="I17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J17" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="I18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J18" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="I19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="J19" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="I20" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="J20" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="I21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="J21" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="I22" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="J22" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="I23" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="J23" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="I24" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="J24" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="I25" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="J25" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="I26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="J26" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="I27" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="J27" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="I28" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="J28" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="I29" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="J29" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="I30" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="J30" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="I31" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="J31" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="I32" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="J32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="I33" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="J33" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="I34" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="J34" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="I35" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J35" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="I36" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="J36" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="I37" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="J37" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="I38" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="J38" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="I39" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="J39" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="I40" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="J40" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="I41" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="J41" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="I42" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="J42" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="I43" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="J43" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="I44" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="J44" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="I45" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="J45" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="I46" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="J46" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="I47" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="J47" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="I48" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="J48" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="I49" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="J49" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="I50" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="J50" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="I51" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="J51" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="I52" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="J52" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="I53" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="J53" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="I54" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="J54" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="I55" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="J55" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="I56" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="J56" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="I57" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="J57" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="I58" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="J58" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="I60" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="J60" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="I61" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="J61" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="I62" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="J62" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="I63" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="J63" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="I64" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="J64" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="I65" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="J65" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="I66" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="J66" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="I67" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="J67" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="I68" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="J68" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>